<commit_message>
fixed data analysis sidebar
</commit_message>
<xml_diff>
--- a/Machine_Learning/stfy_importance.xlsx
+++ b/Machine_Learning/stfy_importance.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.002485676441724692</v>
+        <v>0.005438786316491882</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.05148273620613204</v>
+        <v>0.05968737632435654</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.02928276293509106</v>
+        <v>0.02419491912793581</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.03744162191541218</v>
+        <v>0.03621861882594592</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1729657569689406</v>
+        <v>0.1554086597736452</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0629656286375254</v>
+        <v>0.05801805089369379</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1049269111650992</v>
+        <v>0.1230389365061619</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.03890919042561979</v>
+        <v>0.03967146056162398</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1908908144230645</v>
+        <v>0.1839243143310103</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.02399704327336724</v>
+        <v>0.01897628365072135</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.04400648530640743</v>
+        <v>0.03493978196040689</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.03129804788156804</v>
+        <v>0.02546352325793216</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.02958094838044464</v>
+        <v>0.02533537266980946</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.01667248556912273</v>
+        <v>0.02346693498438158</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.0246701860617276</v>
+        <v>0.03139293223836195</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.03207021076165161</v>
+        <v>0.02559912392072757</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.009721465020856215</v>
+        <v>0.006638500410475031</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.0201934485541647</v>
+        <v>0.02814984173776284</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.020121370493189</v>
+        <v>0.02522989868018976</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.0008944526662795781</v>
+        <v>0.005011118523811611</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.007105258107457961</v>
+        <v>0.01568976138265739</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.009414082011935073</v>
+        <v>0.006219801865620575</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.01269961184465755</v>
+        <v>0.0154825700666057</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.007571423528619508</v>
+        <v>0.0102661265955363</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.01863238141994174</v>
+        <v>0.01653730539413442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>